<commit_message>
UT Repairing Scheulde Final
</commit_message>
<xml_diff>
--- a/UT Repairing Schedule.xlsx
+++ b/UT Repairing Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\DESKTOP-VNHB2O6\MDYInternShip\Documentation Format\21-7-2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF9CF57-B7C6-40BD-B87B-13E8AAA8EB77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F63648-D745-429A-A40A-8525E26DC8A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="558" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="114">
   <si>
     <t>Process Brief</t>
   </si>
@@ -642,7 +642,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="169">
+  <cellXfs count="172">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1056,8 +1056,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1086,6 +1086,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1101,14 +1107,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2500,8 +2509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B3B0CDD-AA81-430C-A6F5-5B31D512AC58}">
   <dimension ref="A1:BC24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BB4" sqref="BB4"/>
+    <sheetView tabSelected="1" topLeftCell="C5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Y16" sqref="Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.7109375" defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2908,7 +2917,7 @@
       <c r="BB6" s="87" t="s">
         <v>109</v>
       </c>
-      <c r="BC6" s="166" t="s">
+      <c r="BC6" s="151" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2972,7 +2981,7 @@
       <c r="BA7" s="86">
         <v>0.5</v>
       </c>
-      <c r="BB7" s="167" t="s">
+      <c r="BB7" s="161" t="s">
         <v>109</v>
       </c>
       <c r="BC7" s="74" t="s">
@@ -3037,7 +3046,7 @@
         <v>45860</v>
       </c>
       <c r="BA8" s="104"/>
-      <c r="BB8" s="168"/>
+      <c r="BB8" s="162"/>
       <c r="BC8" s="74" t="s">
         <v>113</v>
       </c>
@@ -3170,7 +3179,9 @@
       <c r="BA10" s="93">
         <v>0.5</v>
       </c>
-      <c r="BB10" s="45"/>
+      <c r="BB10" s="45" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="11" spans="1:55" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
@@ -3542,7 +3553,7 @@
         <v>45860</v>
       </c>
       <c r="BA16" s="143"/>
-      <c r="BB16" s="65"/>
+      <c r="BB16" s="64"/>
     </row>
     <row r="17" spans="1:54" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -3605,10 +3616,12 @@
       <c r="AZ17" s="146">
         <v>45860</v>
       </c>
-      <c r="BA17" s="93">
+      <c r="BA17" s="168">
         <v>0.5</v>
       </c>
-      <c r="BB17" s="65"/>
+      <c r="BB17" s="170" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="18" spans="1:54" s="2" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -3671,8 +3684,8 @@
       <c r="AZ18" s="146">
         <v>45860</v>
       </c>
-      <c r="BA18" s="144"/>
-      <c r="BB18" s="65"/>
+      <c r="BA18" s="169"/>
+      <c r="BB18" s="171"/>
     </row>
     <row r="19" spans="1:54" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F19" s="31" t="s">
@@ -3733,7 +3746,7 @@
       <c r="BA19" s="93">
         <v>1.5</v>
       </c>
-      <c r="BB19" s="23"/>
+      <c r="BB19" s="29"/>
     </row>
     <row r="20" spans="1:54" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F20" s="31" t="s">
@@ -3907,7 +3920,7 @@
       <c r="AZ22" s="149">
         <v>45860</v>
       </c>
-      <c r="BA22" s="151">
+      <c r="BA22" s="126">
         <v>0.5</v>
       </c>
       <c r="BB22" s="23"/>
@@ -4031,7 +4044,8 @@
       <c r="BB24" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="BB17:BB18"/>
     <mergeCell ref="F1:R1"/>
     <mergeCell ref="S1:AV1"/>
     <mergeCell ref="AW1:AY1"/>
@@ -5281,58 +5295,58 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="161" t="s">
+      <c r="F1" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="161"/>
-      <c r="P1" s="161"/>
-      <c r="Q1" s="161"/>
-      <c r="R1" s="161"/>
-      <c r="S1" s="162" t="s">
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
-      <c r="AF1" s="162"/>
-      <c r="AG1" s="162"/>
-      <c r="AH1" s="162"/>
-      <c r="AI1" s="162"/>
-      <c r="AJ1" s="162"/>
-      <c r="AK1" s="162"/>
-      <c r="AL1" s="162"/>
-      <c r="AM1" s="162"/>
-      <c r="AN1" s="162"/>
-      <c r="AO1" s="162"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
+      <c r="T1" s="164"/>
+      <c r="U1" s="164"/>
+      <c r="V1" s="164"/>
+      <c r="W1" s="164"/>
+      <c r="X1" s="164"/>
+      <c r="Y1" s="164"/>
+      <c r="Z1" s="164"/>
+      <c r="AA1" s="164"/>
+      <c r="AB1" s="164"/>
+      <c r="AC1" s="164"/>
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="164"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+      <c r="AS1" s="164"/>
+      <c r="AT1" s="164"/>
+      <c r="AU1" s="164"/>
       <c r="AV1" s="155"/>
-      <c r="AW1" s="162" t="s">
+      <c r="AW1" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="AX1" s="162"/>
-      <c r="AY1" s="162"/>
+      <c r="AX1" s="164"/>
+      <c r="AY1" s="164"/>
       <c r="AZ1" s="128" t="s">
         <v>4</v>
       </c>
@@ -6641,58 +6655,58 @@
   </cols>
   <sheetData>
     <row r="1" spans="6:59" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F1" s="164" t="s">
+      <c r="F1" s="166" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="164"/>
-      <c r="H1" s="164"/>
-      <c r="I1" s="164"/>
-      <c r="J1" s="164"/>
-      <c r="K1" s="164"/>
-      <c r="L1" s="164"/>
-      <c r="M1" s="164"/>
-      <c r="N1" s="164"/>
-      <c r="O1" s="164"/>
-      <c r="P1" s="164"/>
-      <c r="Q1" s="164"/>
-      <c r="R1" s="164"/>
-      <c r="S1" s="163" t="s">
+      <c r="G1" s="166"/>
+      <c r="H1" s="166"/>
+      <c r="I1" s="166"/>
+      <c r="J1" s="166"/>
+      <c r="K1" s="166"/>
+      <c r="L1" s="166"/>
+      <c r="M1" s="166"/>
+      <c r="N1" s="166"/>
+      <c r="O1" s="166"/>
+      <c r="P1" s="166"/>
+      <c r="Q1" s="166"/>
+      <c r="R1" s="166"/>
+      <c r="S1" s="165" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="163"/>
-      <c r="U1" s="163"/>
-      <c r="V1" s="163"/>
-      <c r="W1" s="163"/>
-      <c r="X1" s="163"/>
-      <c r="Y1" s="163"/>
-      <c r="Z1" s="163"/>
-      <c r="AA1" s="163"/>
-      <c r="AB1" s="163"/>
-      <c r="AC1" s="163"/>
-      <c r="AD1" s="163"/>
-      <c r="AE1" s="163"/>
-      <c r="AF1" s="163"/>
-      <c r="AG1" s="163"/>
-      <c r="AH1" s="163"/>
-      <c r="AI1" s="163"/>
-      <c r="AJ1" s="163"/>
-      <c r="AK1" s="163"/>
-      <c r="AL1" s="163"/>
-      <c r="AM1" s="163"/>
-      <c r="AN1" s="163"/>
-      <c r="AO1" s="163"/>
-      <c r="AP1" s="163"/>
-      <c r="AQ1" s="163"/>
-      <c r="AR1" s="163"/>
-      <c r="AS1" s="163"/>
-      <c r="AT1" s="163"/>
-      <c r="AU1" s="163"/>
-      <c r="AV1" s="165"/>
-      <c r="AW1" s="163" t="s">
+      <c r="T1" s="165"/>
+      <c r="U1" s="165"/>
+      <c r="V1" s="165"/>
+      <c r="W1" s="165"/>
+      <c r="X1" s="165"/>
+      <c r="Y1" s="165"/>
+      <c r="Z1" s="165"/>
+      <c r="AA1" s="165"/>
+      <c r="AB1" s="165"/>
+      <c r="AC1" s="165"/>
+      <c r="AD1" s="165"/>
+      <c r="AE1" s="165"/>
+      <c r="AF1" s="165"/>
+      <c r="AG1" s="165"/>
+      <c r="AH1" s="165"/>
+      <c r="AI1" s="165"/>
+      <c r="AJ1" s="165"/>
+      <c r="AK1" s="165"/>
+      <c r="AL1" s="165"/>
+      <c r="AM1" s="165"/>
+      <c r="AN1" s="165"/>
+      <c r="AO1" s="165"/>
+      <c r="AP1" s="165"/>
+      <c r="AQ1" s="165"/>
+      <c r="AR1" s="165"/>
+      <c r="AS1" s="165"/>
+      <c r="AT1" s="165"/>
+      <c r="AU1" s="165"/>
+      <c r="AV1" s="167"/>
+      <c r="AW1" s="165" t="s">
         <v>20</v>
       </c>
-      <c r="AX1" s="163"/>
-      <c r="AY1" s="163"/>
+      <c r="AX1" s="165"/>
+      <c r="AY1" s="165"/>
       <c r="AZ1" s="72" t="s">
         <v>4</v>
       </c>
@@ -8017,58 +8031,58 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="161" t="s">
+      <c r="F1" s="163" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="161"/>
-      <c r="H1" s="161"/>
-      <c r="I1" s="161"/>
-      <c r="J1" s="161"/>
-      <c r="K1" s="161"/>
-      <c r="L1" s="161"/>
-      <c r="M1" s="161"/>
-      <c r="N1" s="161"/>
-      <c r="O1" s="161"/>
-      <c r="P1" s="161"/>
-      <c r="Q1" s="161"/>
-      <c r="R1" s="161"/>
-      <c r="S1" s="162" t="s">
+      <c r="G1" s="163"/>
+      <c r="H1" s="163"/>
+      <c r="I1" s="163"/>
+      <c r="J1" s="163"/>
+      <c r="K1" s="163"/>
+      <c r="L1" s="163"/>
+      <c r="M1" s="163"/>
+      <c r="N1" s="163"/>
+      <c r="O1" s="163"/>
+      <c r="P1" s="163"/>
+      <c r="Q1" s="163"/>
+      <c r="R1" s="163"/>
+      <c r="S1" s="164" t="s">
         <v>0</v>
       </c>
-      <c r="T1" s="162"/>
-      <c r="U1" s="162"/>
-      <c r="V1" s="162"/>
-      <c r="W1" s="162"/>
-      <c r="X1" s="162"/>
-      <c r="Y1" s="162"/>
-      <c r="Z1" s="162"/>
-      <c r="AA1" s="162"/>
-      <c r="AB1" s="162"/>
-      <c r="AC1" s="162"/>
-      <c r="AD1" s="162"/>
-      <c r="AE1" s="162"/>
-      <c r="AF1" s="162"/>
-      <c r="AG1" s="162"/>
-      <c r="AH1" s="162"/>
-      <c r="AI1" s="162"/>
-      <c r="AJ1" s="162"/>
-      <c r="AK1" s="162"/>
-      <c r="AL1" s="162"/>
-      <c r="AM1" s="162"/>
-      <c r="AN1" s="162"/>
-      <c r="AO1" s="162"/>
-      <c r="AP1" s="162"/>
-      <c r="AQ1" s="162"/>
-      <c r="AR1" s="162"/>
-      <c r="AS1" s="162"/>
-      <c r="AT1" s="162"/>
-      <c r="AU1" s="162"/>
+      <c r="T1" s="164"/>
+      <c r="U1" s="164"/>
+      <c r="V1" s="164"/>
+      <c r="W1" s="164"/>
+      <c r="X1" s="164"/>
+      <c r="Y1" s="164"/>
+      <c r="Z1" s="164"/>
+      <c r="AA1" s="164"/>
+      <c r="AB1" s="164"/>
+      <c r="AC1" s="164"/>
+      <c r="AD1" s="164"/>
+      <c r="AE1" s="164"/>
+      <c r="AF1" s="164"/>
+      <c r="AG1" s="164"/>
+      <c r="AH1" s="164"/>
+      <c r="AI1" s="164"/>
+      <c r="AJ1" s="164"/>
+      <c r="AK1" s="164"/>
+      <c r="AL1" s="164"/>
+      <c r="AM1" s="164"/>
+      <c r="AN1" s="164"/>
+      <c r="AO1" s="164"/>
+      <c r="AP1" s="164"/>
+      <c r="AQ1" s="164"/>
+      <c r="AR1" s="164"/>
+      <c r="AS1" s="164"/>
+      <c r="AT1" s="164"/>
+      <c r="AU1" s="164"/>
       <c r="AV1" s="155"/>
-      <c r="AW1" s="162" t="s">
+      <c r="AW1" s="164" t="s">
         <v>20</v>
       </c>
-      <c r="AX1" s="162"/>
-      <c r="AY1" s="162"/>
+      <c r="AX1" s="164"/>
+      <c r="AY1" s="164"/>
       <c r="AZ1" s="128" t="s">
         <v>4</v>
       </c>

</xml_diff>